<commit_message>
Altera tempo de animação index
</commit_message>
<xml_diff>
--- a/Documentação/Sprint-1/Requisitos - ADS.xlsx
+++ b/Documentação/Sprint-1/Requisitos - ADS.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guimi\OneDrive\Área de Trabalho\Segundo semestre\Pesquisa e Inovação\Illumy\Documentação\Sprint-1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_B728D0D37E5374DD123F53A2BD1EA2B7B3A911D2" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8640" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Histórico de Alterações" sheetId="4" r:id="rId1"/>
@@ -458,7 +464,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22">
     <font>
       <sz val="10"/>
@@ -1120,6 +1126,12 @@
     <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1191,12 +1203,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1204,54 +1210,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="22">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Exo 2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Exo 2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1612,10 +1570,58 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Exo 2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Exo 2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -1648,7 +1654,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1" descr="logo"/>
+        <xdr:cNvPr id="2" name="Imagem 1" descr="logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1692,27 +1704,27 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="D7:U91" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="21" tableBorderDxfId="20">
-  <autoFilter ref="D7:U91"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabela2" displayName="Tabela2" ref="D7:U91" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="D7:U91" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
-    <tableColumn id="1" name="Descrição do Requisito" dataDxfId="19"/>
-    <tableColumn id="2" name="Objetivo / Estratégia de Negócio" dataDxfId="18"/>
-    <tableColumn id="3" name="Prioridade" dataDxfId="17"/>
-    <tableColumn id="4" name="Versão do Requisito" dataDxfId="16"/>
-    <tableColumn id="7" name="Tipo Requisito " dataDxfId="15"/>
-    <tableColumn id="8" name="Complexidade" dataDxfId="14"/>
-    <tableColumn id="9" name="Solicitante" dataDxfId="13"/>
-    <tableColumn id="10" name="Responsável" dataDxfId="12"/>
-    <tableColumn id="11" name="Validador" dataDxfId="11"/>
-    <tableColumn id="12" name="Critérios de Aceitação" dataDxfId="10"/>
-    <tableColumn id="13" name="Dependência Internas entre Requisitos  (rastreabilidade)" dataDxfId="9"/>
-    <tableColumn id="14" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="8"/>
-    <tableColumn id="15" name="Data da Criação" dataDxfId="7"/>
-    <tableColumn id="16" name="Data Última Alteração" dataDxfId="6"/>
-    <tableColumn id="17" name="Responsável pela última alteração" dataDxfId="5"/>
-    <tableColumn id="18" name="Motivo Última Alteração" dataDxfId="4"/>
-    <tableColumn id="19" name="Documentação de Apoio" dataDxfId="3"/>
-    <tableColumn id="20" name="Situação do Requisito" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Descrição do Requisito" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Prioridade" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Versão do Requisito" dataDxfId="14"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Tipo Requisito " dataDxfId="13"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Complexidade" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Solicitante" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Responsável" dataDxfId="10"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Validador" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Critérios de Aceitação" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Dependência Internas entre Requisitos  (rastreabilidade)" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Dependências Externas entre Requisitos (Rastreabilidade)" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Data da Criação" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Data Última Alteração" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Responsável pela última alteração" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Motivo Última Alteração" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Documentação de Apoio" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Situação do Requisito" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1721,7 +1733,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1759,9 +1771,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1794,9 +1806,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1829,9 +1858,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2004,31 +2050,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="32.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
     </row>
     <row r="4" spans="2:5" ht="27" customHeight="1">
       <c r="B4" s="6" t="s">
@@ -2044,7 +2090,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:5" ht="15">
+    <row r="5" spans="2:5" ht="14.4">
       <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
@@ -2054,43 +2100,43 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="2:5" ht="15">
+    <row r="6" spans="2:5" ht="14.4">
       <c r="B6" s="4"/>
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="2:5" ht="15">
+    <row r="7" spans="2:5" ht="14.4">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="2:5" ht="15">
+    <row r="8" spans="2:5" ht="14.4">
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="2:5" ht="15">
+    <row r="9" spans="2:5" ht="14.4">
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="2:5" ht="15">
+    <row r="10" spans="2:5" ht="14.4">
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="2:5" ht="15">
+    <row r="11" spans="2:5" ht="14.4">
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="2:5" ht="15">
+    <row r="12" spans="2:5" ht="14.4">
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="4"/>
@@ -2124,41 +2170,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:V92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="4" ySplit="7" topLeftCell="I29" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="4" ySplit="7" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="O32" sqref="O32"/>
+      <selection pane="bottomRight" activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" style="50" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" style="50" customWidth="1"/>
-    <col min="11" max="11" width="20.5703125" style="50" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="50" customWidth="1"/>
-    <col min="13" max="13" width="26.140625" style="50" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="30.5703125" style="50" customWidth="1"/>
+    <col min="1" max="1" width="2.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="3.88671875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="29.5546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="19.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" style="50" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" style="50" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" style="50" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="50" customWidth="1"/>
+    <col min="13" max="13" width="26.109375" style="50" customWidth="1"/>
+    <col min="14" max="14" width="22.44140625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="30.5546875" style="50" customWidth="1"/>
     <col min="16" max="16" width="16" style="50" customWidth="1"/>
-    <col min="17" max="17" width="14.7109375" style="50" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="50" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16" style="7" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="25.42578125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="14.42578125" style="7" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="7"/>
+    <col min="20" max="20" width="16.109375" style="7" customWidth="1"/>
+    <col min="21" max="21" width="25.44140625" style="7" customWidth="1"/>
+    <col min="22" max="22" width="14.44140625" style="7" customWidth="1"/>
+    <col min="23" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="14.25" customHeight="1" thickBot="1">
@@ -2182,22 +2228,22 @@
       <c r="U1" s="12"/>
     </row>
     <row r="2" spans="2:22" ht="16.5" customHeight="1" thickBot="1">
-      <c r="E2" s="65" t="s">
+      <c r="E2" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="71" t="s">
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="P2" s="71"/>
+      <c r="P2" s="73"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="16"/>
       <c r="T2" s="17" t="s">
@@ -2206,40 +2252,40 @@
       <c r="U2" s="12"/>
     </row>
     <row r="3" spans="2:22" ht="14.25" customHeight="1" thickBot="1">
-      <c r="E3" s="68"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="70"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="73"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="75"/>
       <c r="Q3" s="7"/>
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
       <c r="U3" s="18"/>
     </row>
     <row r="4" spans="2:22" ht="12.75" customHeight="1" thickBot="1">
-      <c r="E4" s="56" t="s">
+      <c r="E4" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="74" t="s">
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="P4" s="74"/>
+      <c r="P4" s="76"/>
       <c r="Q4" s="12"/>
       <c r="S4" s="18"/>
       <c r="T4" s="19"/>
@@ -2248,18 +2294,18 @@
     <row r="5" spans="2:22">
       <c r="B5" s="20"/>
       <c r="D5" s="20"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="60"/>
-      <c r="H5" s="60"/>
-      <c r="I5" s="60"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="60"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="76"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="77"/>
+      <c r="P5" s="78"/>
       <c r="Q5" s="20"/>
       <c r="S5" s="18"/>
       <c r="T5" s="19"/>
@@ -2267,18 +2313,18 @@
     </row>
     <row r="6" spans="2:22" s="21" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
       <c r="C6" s="22"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="63"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="77"/>
-      <c r="P6" s="78"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="79"/>
+      <c r="P6" s="80"/>
       <c r="Q6" s="23"/>
       <c r="S6" s="24"/>
       <c r="T6" s="24"/>
@@ -2347,7 +2393,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="2:22" s="39" customFormat="1" ht="27">
+    <row r="8" spans="2:22" s="39" customFormat="1" ht="27.6">
       <c r="B8" s="32">
         <v>1</v>
       </c>
@@ -2381,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:22" s="39" customFormat="1" ht="40.5">
+    <row r="9" spans="2:22" s="39" customFormat="1" ht="41.4">
       <c r="B9" s="40"/>
       <c r="C9" s="41" t="s">
         <v>26</v>
@@ -2641,7 +2687,7 @@
       <c r="T15" s="34"/>
       <c r="U15" s="36"/>
     </row>
-    <row r="16" spans="2:22" s="39" customFormat="1" ht="40.5">
+    <row r="16" spans="2:22" s="39" customFormat="1" ht="41.4">
       <c r="B16" s="40"/>
       <c r="C16" s="41" t="s">
         <v>35</v>
@@ -2679,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="17" spans="2:21" s="39" customFormat="1" ht="27.6">
       <c r="B17" s="40"/>
       <c r="C17" s="41" t="s">
         <v>43</v>
@@ -2717,7 +2763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="18" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B18" s="40"/>
       <c r="C18" s="41" t="s">
         <v>44</v>
@@ -2755,7 +2801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="19" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B19" s="40"/>
       <c r="C19" s="41" t="s">
         <v>45</v>
@@ -2793,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="20" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B20" s="40"/>
       <c r="C20" s="41" t="s">
         <v>48</v>
@@ -2869,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="22" spans="2:21" s="39" customFormat="1" ht="27.6">
       <c r="B22" s="40"/>
       <c r="C22" s="41" t="s">
         <v>89</v>
@@ -2909,7 +2955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="23" spans="2:21" s="39" customFormat="1" ht="27.6">
       <c r="B23" s="40">
         <v>3</v>
       </c>
@@ -3161,7 +3207,7 @@
       <c r="T29" s="34"/>
       <c r="U29" s="36"/>
     </row>
-    <row r="30" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="30" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B30" s="40"/>
       <c r="C30" s="41" t="s">
         <v>90</v>
@@ -3203,7 +3249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="31" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B31" s="40">
         <v>4</v>
       </c>
@@ -3212,12 +3258,12 @@
         <v>96</v>
       </c>
       <c r="E31" s="35"/>
-      <c r="F31" s="79"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="80"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
       <c r="L31" s="36"/>
       <c r="M31" s="36"/>
       <c r="N31" s="35"/>
@@ -3231,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="32" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B32" s="40"/>
       <c r="C32" s="41" t="s">
         <v>97</v>
@@ -3269,7 +3315,7 @@
       <c r="T32" s="53"/>
       <c r="U32" s="52"/>
     </row>
-    <row r="33" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="33" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B33" s="40"/>
       <c r="C33" s="41" t="s">
         <v>98</v>
@@ -3305,7 +3351,7 @@
       <c r="T33" s="53"/>
       <c r="U33" s="52"/>
     </row>
-    <row r="34" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="34" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B34" s="40">
         <v>5</v>
       </c>
@@ -3335,7 +3381,7 @@
       <c r="T34" s="34"/>
       <c r="U34" s="36"/>
     </row>
-    <row r="35" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="35" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B35" s="40"/>
       <c r="C35" s="41" t="s">
         <v>74</v>
@@ -3375,7 +3421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:21" s="39" customFormat="1" ht="27">
+    <row r="36" spans="2:21" s="39" customFormat="1" ht="27.6">
       <c r="B36" s="40"/>
       <c r="C36" s="41" t="s">
         <v>75</v>
@@ -3413,7 +3459,7 @@
       <c r="T36" s="34"/>
       <c r="U36" s="36"/>
     </row>
-    <row r="37" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="37" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B37" s="40"/>
       <c r="C37" s="41" t="s">
         <v>77</v>
@@ -3451,7 +3497,7 @@
       <c r="T37" s="34"/>
       <c r="U37" s="36"/>
     </row>
-    <row r="38" spans="2:21" s="39" customFormat="1" ht="40.5">
+    <row r="38" spans="2:21" s="39" customFormat="1" ht="41.4">
       <c r="B38" s="40">
         <v>6</v>
       </c>
@@ -3489,7 +3535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="39" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B39" s="40">
         <v>10</v>
       </c>
@@ -3515,7 +3561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="40" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B40" s="40">
         <v>11</v>
       </c>
@@ -3541,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="41" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B41" s="40">
         <v>12</v>
       </c>
@@ -3567,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="42" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B42" s="40">
         <v>13</v>
       </c>
@@ -3593,7 +3639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="43" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B43" s="40">
         <v>13</v>
       </c>
@@ -3619,7 +3665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="44" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B44" s="40">
         <v>14</v>
       </c>
@@ -3645,7 +3691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="45" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B45" s="40">
         <v>15</v>
       </c>
@@ -3671,7 +3717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="46" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B46" s="40">
         <v>16</v>
       </c>
@@ -3697,7 +3743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="47" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B47" s="40">
         <v>17</v>
       </c>
@@ -3723,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="48" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B48" s="40">
         <v>18</v>
       </c>
@@ -3749,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="49" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B49" s="40">
         <v>19</v>
       </c>
@@ -3775,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="50" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B50" s="40">
         <v>20</v>
       </c>
@@ -3801,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="51" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B51" s="40">
         <v>21</v>
       </c>
@@ -3827,7 +3873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="52" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B52" s="40">
         <v>22</v>
       </c>
@@ -3853,7 +3899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="53" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B53" s="40">
         <v>23</v>
       </c>
@@ -3879,7 +3925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="54" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B54" s="40">
         <v>24</v>
       </c>
@@ -3905,7 +3951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="55" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B55" s="40">
         <v>25</v>
       </c>
@@ -3931,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="56" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B56" s="40">
         <v>26</v>
       </c>
@@ -3957,7 +4003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="57" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B57" s="40">
         <v>27</v>
       </c>
@@ -3983,7 +4029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="58" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B58" s="40">
         <v>28</v>
       </c>
@@ -4009,7 +4055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="59" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B59" s="40">
         <v>29</v>
       </c>
@@ -4035,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="60" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B60" s="40">
         <v>30</v>
       </c>
@@ -4061,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="61" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B61" s="40">
         <v>31</v>
       </c>
@@ -4087,7 +4133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="62" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B62" s="40">
         <v>32</v>
       </c>
@@ -4113,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="63" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B63" s="40">
         <v>33</v>
       </c>
@@ -4139,7 +4185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="64" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B64" s="40">
         <v>34</v>
       </c>
@@ -4165,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="65" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B65" s="40">
         <v>35</v>
       </c>
@@ -4191,7 +4237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="66" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B66" s="40">
         <v>36</v>
       </c>
@@ -4217,7 +4263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="67" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B67" s="40">
         <v>37</v>
       </c>
@@ -4243,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="68" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B68" s="40">
         <v>38</v>
       </c>
@@ -4269,7 +4315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="69" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B69" s="40">
         <v>39</v>
       </c>
@@ -4295,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="70" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B70" s="40">
         <v>40</v>
       </c>
@@ -4321,7 +4367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="71" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B71" s="40">
         <v>41</v>
       </c>
@@ -4347,7 +4393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="72" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B72" s="40">
         <v>42</v>
       </c>
@@ -4373,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="73" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B73" s="40">
         <v>43</v>
       </c>
@@ -4399,7 +4445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="74" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B74" s="40">
         <v>44</v>
       </c>
@@ -4425,7 +4471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="75" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B75" s="40">
         <v>45</v>
       </c>
@@ -4451,7 +4497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="76" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B76" s="40">
         <v>46</v>
       </c>
@@ -4477,7 +4523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="77" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B77" s="40">
         <v>47</v>
       </c>
@@ -4503,7 +4549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="78" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B78" s="40">
         <v>48</v>
       </c>
@@ -4529,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="79" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B79" s="40">
         <v>49</v>
       </c>
@@ -4555,7 +4601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="80" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B80" s="40">
         <v>50</v>
       </c>
@@ -4581,7 +4627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="81" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B81" s="40">
         <v>51</v>
       </c>
@@ -4607,7 +4653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="82" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B82" s="40">
         <v>52</v>
       </c>
@@ -4633,7 +4679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="83" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B83" s="40">
         <v>53</v>
       </c>
@@ -4659,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="84" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B84" s="40">
         <v>54</v>
       </c>
@@ -4685,7 +4731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="85" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B85" s="40">
         <v>55</v>
       </c>
@@ -4711,7 +4757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="86" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B86" s="40">
         <v>56</v>
       </c>
@@ -4737,7 +4783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="87" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B87" s="40">
         <v>57</v>
       </c>
@@ -4763,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="88" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B88" s="40">
         <v>58</v>
       </c>
@@ -4789,7 +4835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="89" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B89" s="40">
         <v>59</v>
       </c>
@@ -4815,7 +4861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:21" s="39" customFormat="1" ht="15.75">
+    <row r="90" spans="2:21" s="39" customFormat="1" ht="14.4">
       <c r="B90" s="40">
         <v>60</v>
       </c>
@@ -4841,7 +4887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:21" s="39" customFormat="1" ht="16.5" thickBot="1">
+    <row r="91" spans="2:21" s="39" customFormat="1" ht="15" thickBot="1">
       <c r="B91" s="43">
         <v>61</v>
       </c>
@@ -4881,13 +4927,13 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U91">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U8:U91" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I32:I91 I8:I30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I32:I91 I8:I30" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H91 H8:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H32:H91 H8:H30" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>$T$1:$T$6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>